<commit_message>
Added further details and the ordering
</commit_message>
<xml_diff>
--- a/generated_data/Nov2025_Rollover_Data.xlsx
+++ b/generated_data/Nov2025_Rollover_Data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="254">
   <si>
     <t>Sectoral Index</t>
   </si>
@@ -762,6 +762,24 @@
   </si>
   <si>
     <t>Long Unwind (MoM- , %Roll- , Cost-)</t>
+  </si>
+  <si>
+    <t>Current Date</t>
+  </si>
+  <si>
+    <t>251125</t>
+  </si>
+  <si>
+    <t>Prev Date</t>
+  </si>
+  <si>
+    <t>281025</t>
+  </si>
+  <si>
+    <t>Next Date</t>
+  </si>
+  <si>
+    <t>301225</t>
   </si>
 </sst>
 </file>
@@ -1232,15 +1250,33 @@
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -9868,16 +9904,34 @@
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>246</v>
       </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
@@ -9927,40 +9981,40 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="C6">
-        <v>6081.5</v>
+        <v>5833</v>
       </c>
       <c r="D6">
-        <v>6110.5</v>
+        <v>5875.5</v>
       </c>
       <c r="E6">
-        <v>29</v>
+        <v>42.5</v>
       </c>
       <c r="F6">
-        <v>94.37</v>
+        <v>95.62</v>
       </c>
       <c r="G6">
-        <v>90.15000000000001</v>
+        <v>94.42</v>
       </c>
       <c r="H6">
-        <v>0.41</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I6">
-        <v>-0.25</v>
+        <v>-0.12</v>
       </c>
       <c r="J6">
-        <v>4.22</v>
+        <v>1.2</v>
       </c>
       <c r="K6">
-        <v>0.66</v>
+        <v>0.8</v>
       </c>
       <c r="L6">
-        <v>8.41</v>
+        <v>4.24</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -9971,37 +10025,37 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7">
-        <v>110.21</v>
+        <v>6081.5</v>
       </c>
       <c r="D7">
-        <v>110.99</v>
+        <v>6110.5</v>
       </c>
       <c r="E7">
-        <v>0.78</v>
+        <v>29</v>
       </c>
       <c r="F7">
-        <v>96.47</v>
+        <v>94.37</v>
       </c>
       <c r="G7">
-        <v>96.2</v>
+        <v>90.15000000000001</v>
       </c>
       <c r="H7">
-        <v>0.64</v>
+        <v>0.41</v>
       </c>
       <c r="I7">
-        <v>0.5600000000000001</v>
+        <v>-0.25</v>
       </c>
       <c r="J7">
-        <v>0.27</v>
+        <v>4.22</v>
       </c>
       <c r="K7">
-        <v>0.08</v>
+        <v>0.66</v>
       </c>
       <c r="L7">
-        <v>3.02</v>
+        <v>8.41</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -10009,40 +10063,40 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>146</v>
       </c>
       <c r="C8">
-        <v>1285.3</v>
+        <v>1530.6</v>
       </c>
       <c r="D8">
-        <v>1292.4</v>
+        <v>1538.9</v>
       </c>
       <c r="E8">
-        <v>7.1</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F8">
-        <v>97.28</v>
+        <v>96.36</v>
       </c>
       <c r="G8">
-        <v>92.97</v>
+        <v>92.47</v>
       </c>
       <c r="H8">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="I8">
-        <v>0.47</v>
+        <v>0.04</v>
       </c>
       <c r="J8">
-        <v>4.32</v>
+        <v>3.89</v>
       </c>
       <c r="K8">
-        <v>0.23</v>
+        <v>0.53</v>
       </c>
       <c r="L8">
-        <v>7</v>
+        <v>2.03</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -10050,40 +10104,40 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C9">
-        <v>839.9</v>
+        <v>355.85</v>
       </c>
       <c r="D9">
-        <v>844.05</v>
+        <v>357.9</v>
       </c>
       <c r="E9">
-        <v>4.15</v>
+        <v>2.05</v>
       </c>
       <c r="F9">
-        <v>93.55</v>
+        <v>92.8</v>
       </c>
       <c r="G9">
-        <v>92.61</v>
+        <v>82.70999999999999</v>
       </c>
       <c r="H9">
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
       <c r="I9">
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
       <c r="J9">
-        <v>0.9399999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="K9">
-        <v>0.13</v>
+        <v>0.47</v>
       </c>
       <c r="L9">
-        <v>5.02</v>
+        <v>4.46</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -10091,40 +10145,40 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="C10">
-        <v>570.35</v>
+        <v>749.7</v>
       </c>
       <c r="D10">
-        <v>573.4</v>
+        <v>755.45</v>
       </c>
       <c r="E10">
-        <v>3.05</v>
+        <v>5.75</v>
       </c>
       <c r="F10">
-        <v>95.97</v>
+        <v>95.29000000000001</v>
       </c>
       <c r="G10">
-        <v>94.58</v>
+        <v>94.01000000000001</v>
       </c>
       <c r="H10">
-        <v>0.6899999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="I10">
-        <v>0.63</v>
+        <v>0.36</v>
       </c>
       <c r="J10">
-        <v>1.39</v>
+        <v>1.28</v>
       </c>
       <c r="K10">
-        <v>0.07000000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="L10">
-        <v>0.89</v>
+        <v>6.7</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -10132,40 +10186,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="C11">
-        <v>3855.1</v>
+        <v>1601.1</v>
       </c>
       <c r="D11">
-        <v>3881.6</v>
+        <v>1610.2</v>
       </c>
       <c r="E11">
-        <v>26.5</v>
+        <v>9.1</v>
       </c>
       <c r="F11">
-        <v>94.91</v>
+        <v>96.44</v>
       </c>
       <c r="G11">
-        <v>93.59999999999999</v>
+        <v>93.89</v>
       </c>
       <c r="H11">
-        <v>0.58</v>
+        <v>0.76</v>
       </c>
       <c r="I11">
-        <v>0.48</v>
+        <v>0.33</v>
       </c>
       <c r="J11">
-        <v>1.31</v>
+        <v>2.55</v>
       </c>
       <c r="K11">
-        <v>0.1</v>
+        <v>0.42</v>
       </c>
       <c r="L11">
-        <v>3.72</v>
+        <v>5.19</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -10173,40 +10227,40 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C12">
-        <v>1483.9</v>
+        <v>731.35</v>
       </c>
       <c r="D12">
-        <v>1492.1</v>
+        <v>736.9</v>
       </c>
       <c r="E12">
-        <v>8.199999999999999</v>
+        <v>5.55</v>
       </c>
       <c r="F12">
-        <v>96.87</v>
+        <v>98.78</v>
       </c>
       <c r="G12">
-        <v>94.15000000000001</v>
+        <v>96.95999999999999</v>
       </c>
       <c r="H12">
-        <v>0.74</v>
+        <v>0.77</v>
       </c>
       <c r="I12">
-        <v>0.52</v>
+        <v>0.35</v>
       </c>
       <c r="J12">
-        <v>2.73</v>
+        <v>1.82</v>
       </c>
       <c r="K12">
-        <v>0.22</v>
+        <v>0.42</v>
       </c>
       <c r="L12">
-        <v>4.65</v>
+        <v>1.57</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -10214,40 +10268,40 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="C13">
-        <v>971.5</v>
+        <v>253.97</v>
       </c>
       <c r="D13">
-        <v>977.15</v>
+        <v>255.7</v>
       </c>
       <c r="E13">
-        <v>5.65</v>
+        <v>1.73</v>
       </c>
       <c r="F13">
-        <v>98.44</v>
+        <v>93.29000000000001</v>
       </c>
       <c r="G13">
-        <v>96.68000000000001</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="H13">
-        <v>0.65</v>
+        <v>0.78</v>
       </c>
       <c r="I13">
-        <v>0.63</v>
+        <v>0.39</v>
       </c>
       <c r="J13">
-        <v>1.76</v>
+        <v>1.72</v>
       </c>
       <c r="K13">
-        <v>0.02</v>
+        <v>0.39</v>
       </c>
       <c r="L13">
-        <v>5.46</v>
+        <v>7.27</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -10255,40 +10309,40 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>207</v>
       </c>
       <c r="C14">
-        <v>1011.6</v>
+        <v>5701</v>
       </c>
       <c r="D14">
-        <v>1017.3</v>
+        <v>5729.5</v>
       </c>
       <c r="E14">
-        <v>5.7</v>
+        <v>28.5</v>
       </c>
       <c r="F14">
-        <v>94.45</v>
+        <v>97.06999999999999</v>
       </c>
       <c r="G14">
-        <v>94.18000000000001</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="H14">
-        <v>0.75</v>
+        <v>0.59</v>
       </c>
       <c r="I14">
-        <v>0.67</v>
+        <v>0.22</v>
       </c>
       <c r="J14">
-        <v>0.26</v>
+        <v>3.22</v>
       </c>
       <c r="K14">
-        <v>0.08</v>
+        <v>0.37</v>
       </c>
       <c r="L14">
-        <v>0.74</v>
+        <v>4.95</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -10296,40 +10350,40 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C15">
-        <v>355.85</v>
+        <v>1144.5</v>
       </c>
       <c r="D15">
-        <v>357.9</v>
+        <v>1151.6</v>
       </c>
       <c r="E15">
-        <v>2.05</v>
+        <v>7.1</v>
       </c>
       <c r="F15">
-        <v>92.8</v>
+        <v>90.64</v>
       </c>
       <c r="G15">
-        <v>82.70999999999999</v>
+        <v>88.86</v>
       </c>
       <c r="H15">
-        <v>0.7</v>
+        <v>0.61</v>
       </c>
       <c r="I15">
         <v>0.24</v>
       </c>
       <c r="J15">
-        <v>10.1</v>
+        <v>1.78</v>
       </c>
       <c r="K15">
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
       <c r="L15">
-        <v>4.46</v>
+        <v>2.6</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -10337,40 +10391,40 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="C16">
-        <v>1293</v>
+        <v>3119.2</v>
       </c>
       <c r="D16">
-        <v>1298.5</v>
+        <v>3135.5</v>
       </c>
       <c r="E16">
-        <v>5.5</v>
+        <v>16.3</v>
       </c>
       <c r="F16">
-        <v>94.48</v>
+        <v>97.06999999999999</v>
       </c>
       <c r="G16">
-        <v>89.70999999999999</v>
+        <v>93.06</v>
       </c>
       <c r="H16">
-        <v>0.7</v>
+        <v>0.73</v>
       </c>
       <c r="I16">
-        <v>0.54</v>
+        <v>0.37</v>
       </c>
       <c r="J16">
-        <v>4.77</v>
+        <v>4.01</v>
       </c>
       <c r="K16">
-        <v>0.17</v>
+        <v>0.36</v>
       </c>
       <c r="L16">
-        <v>1.24</v>
+        <v>2</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -10378,40 +10432,40 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C17">
-        <v>1144.5</v>
+        <v>1697.9</v>
       </c>
       <c r="D17">
-        <v>1151.6</v>
+        <v>1710.1</v>
       </c>
       <c r="E17">
-        <v>7.1</v>
+        <v>12.2</v>
       </c>
       <c r="F17">
-        <v>90.64</v>
+        <v>95.22</v>
       </c>
       <c r="G17">
-        <v>88.86</v>
+        <v>88.31999999999999</v>
       </c>
       <c r="H17">
-        <v>0.61</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="I17">
-        <v>0.24</v>
+        <v>0.48</v>
       </c>
       <c r="J17">
-        <v>1.78</v>
+        <v>6.89</v>
       </c>
       <c r="K17">
-        <v>0.37</v>
+        <v>0.32</v>
       </c>
       <c r="L17">
-        <v>2.6</v>
+        <v>11.4</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -10419,40 +10473,40 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>232</v>
       </c>
       <c r="C18">
-        <v>731.35</v>
+        <v>230.76</v>
       </c>
       <c r="D18">
-        <v>736.9</v>
+        <v>232.28</v>
       </c>
       <c r="E18">
-        <v>5.55</v>
+        <v>1.52</v>
       </c>
       <c r="F18">
-        <v>98.78</v>
+        <v>96.81</v>
       </c>
       <c r="G18">
-        <v>96.95999999999999</v>
+        <v>92.18000000000001</v>
       </c>
       <c r="H18">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="I18">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="J18">
-        <v>1.82</v>
+        <v>4.64</v>
       </c>
       <c r="K18">
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
       <c r="L18">
-        <v>1.57</v>
+        <v>2.14</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -10460,40 +10514,40 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
       <c r="C19">
-        <v>1177.7</v>
+        <v>455.25</v>
       </c>
       <c r="D19">
-        <v>1183.6</v>
+        <v>458.5</v>
       </c>
       <c r="E19">
-        <v>5.9</v>
+        <v>3.25</v>
       </c>
       <c r="F19">
-        <v>97.88</v>
+        <v>97.48999999999999</v>
       </c>
       <c r="G19">
-        <v>96.76000000000001</v>
+        <v>85.48</v>
       </c>
       <c r="H19">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="I19">
-        <v>0.55</v>
+        <v>0.39</v>
       </c>
       <c r="J19">
-        <v>1.13</v>
+        <v>12.01</v>
       </c>
       <c r="K19">
-        <v>0.11</v>
+        <v>0.27</v>
       </c>
       <c r="L19">
-        <v>0.75</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -10501,40 +10555,40 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="C20">
-        <v>345.45</v>
+        <v>4311.3</v>
       </c>
       <c r="D20">
-        <v>347.1</v>
+        <v>4341.3</v>
       </c>
       <c r="E20">
-        <v>1.65</v>
+        <v>30</v>
       </c>
       <c r="F20">
-        <v>98.36</v>
+        <v>92.25</v>
       </c>
       <c r="G20">
-        <v>95.29000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="H20">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="I20">
-        <v>0.5600000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="J20">
-        <v>3.07</v>
+        <v>1.75</v>
       </c>
       <c r="K20">
-        <v>0.03</v>
+        <v>0.26</v>
       </c>
       <c r="L20">
-        <v>10.51</v>
+        <v>0.6</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -10542,40 +10596,40 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="C21">
-        <v>612.25</v>
+        <v>1831.7</v>
       </c>
       <c r="D21">
-        <v>615.85</v>
+        <v>1843.7</v>
       </c>
       <c r="E21">
-        <v>3.6</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>98.11</v>
+        <v>96.2</v>
       </c>
       <c r="G21">
-        <v>94.04000000000001</v>
+        <v>92.5</v>
       </c>
       <c r="H21">
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="I21">
-        <v>0.54</v>
+        <v>0.45</v>
       </c>
       <c r="J21">
-        <v>4.08</v>
+        <v>3.7</v>
       </c>
       <c r="K21">
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="L21">
-        <v>1.96</v>
+        <v>1.21</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -10583,40 +10637,40 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="C22">
-        <v>279.05</v>
+        <v>1285.3</v>
       </c>
       <c r="D22">
-        <v>281.1</v>
+        <v>1292.4</v>
       </c>
       <c r="E22">
-        <v>2.05</v>
+        <v>7.1</v>
       </c>
       <c r="F22">
-        <v>96.59999999999999</v>
+        <v>97.28</v>
       </c>
       <c r="G22">
-        <v>88.93000000000001</v>
+        <v>92.97</v>
       </c>
       <c r="H22">
-        <v>0.73</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I22">
-        <v>0.57</v>
+        <v>0.47</v>
       </c>
       <c r="J22">
-        <v>7.67</v>
+        <v>4.32</v>
       </c>
       <c r="K22">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
       <c r="L22">
-        <v>0.98</v>
+        <v>7</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -10624,40 +10678,40 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
       <c r="C23">
-        <v>9867</v>
+        <v>1483.9</v>
       </c>
       <c r="D23">
-        <v>9916</v>
+        <v>1492.1</v>
       </c>
       <c r="E23">
-        <v>49</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F23">
-        <v>90.81</v>
+        <v>96.87</v>
       </c>
       <c r="G23">
-        <v>88.48999999999999</v>
+        <v>94.15000000000001</v>
       </c>
       <c r="H23">
-        <v>0.67</v>
+        <v>0.74</v>
       </c>
       <c r="I23">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="J23">
-        <v>2.32</v>
+        <v>2.73</v>
       </c>
       <c r="K23">
-        <v>0.14</v>
+        <v>0.22</v>
       </c>
       <c r="L23">
-        <v>8.23</v>
+        <v>4.65</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -10665,40 +10719,40 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>214</v>
       </c>
       <c r="C24">
-        <v>1697.9</v>
+        <v>977.55</v>
       </c>
       <c r="D24">
-        <v>1710.1</v>
+        <v>982.6</v>
       </c>
       <c r="E24">
-        <v>12.2</v>
+        <v>5.05</v>
       </c>
       <c r="F24">
-        <v>95.22</v>
+        <v>90.29000000000001</v>
       </c>
       <c r="G24">
-        <v>88.31999999999999</v>
+        <v>89.87</v>
       </c>
       <c r="H24">
-        <v>0.8100000000000001</v>
+        <v>0.77</v>
       </c>
       <c r="I24">
-        <v>0.48</v>
+        <v>0.55</v>
       </c>
       <c r="J24">
-        <v>6.89</v>
+        <v>0.42</v>
       </c>
       <c r="K24">
-        <v>0.32</v>
+        <v>0.22</v>
       </c>
       <c r="L24">
-        <v>11.4</v>
+        <v>1.87</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -10706,40 +10760,40 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="C25">
-        <v>838.25</v>
+        <v>3996.7</v>
       </c>
       <c r="D25">
-        <v>843.45</v>
+        <v>4021.3</v>
       </c>
       <c r="E25">
-        <v>5.2</v>
+        <v>24.6</v>
       </c>
       <c r="F25">
-        <v>95.7</v>
+        <v>97.11</v>
       </c>
       <c r="G25">
-        <v>95.58</v>
+        <v>88.88</v>
       </c>
       <c r="H25">
-        <v>0.47</v>
+        <v>0.7</v>
       </c>
       <c r="I25">
-        <v>0.42</v>
+        <v>0.5</v>
       </c>
       <c r="J25">
-        <v>0.12</v>
+        <v>8.23</v>
       </c>
       <c r="K25">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="L25">
-        <v>15.83</v>
+        <v>0.6</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -10747,40 +10801,40 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>235</v>
       </c>
       <c r="C26">
-        <v>1831.7</v>
+        <v>1731.7</v>
       </c>
       <c r="D26">
-        <v>1843.7</v>
+        <v>1739.2</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="F26">
-        <v>96.2</v>
+        <v>95.27</v>
       </c>
       <c r="G26">
-        <v>92.5</v>
+        <v>90.97</v>
       </c>
       <c r="H26">
         <v>0.7</v>
       </c>
       <c r="I26">
-        <v>0.45</v>
+        <v>0.49</v>
       </c>
       <c r="J26">
-        <v>3.7</v>
+        <v>4.29</v>
       </c>
       <c r="K26">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="L26">
-        <v>1.21</v>
+        <v>1.75</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -10788,40 +10842,40 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="C27">
-        <v>1601.1</v>
+        <v>279.05</v>
       </c>
       <c r="D27">
-        <v>1610.2</v>
+        <v>281.1</v>
       </c>
       <c r="E27">
-        <v>9.1</v>
+        <v>2.05</v>
       </c>
       <c r="F27">
-        <v>96.44</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="G27">
-        <v>93.89</v>
+        <v>88.93000000000001</v>
       </c>
       <c r="H27">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="I27">
-        <v>0.33</v>
+        <v>0.57</v>
       </c>
       <c r="J27">
-        <v>2.55</v>
+        <v>7.67</v>
       </c>
       <c r="K27">
-        <v>0.42</v>
+        <v>0.17</v>
       </c>
       <c r="L27">
-        <v>5.19</v>
+        <v>0.98</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -10829,40 +10883,40 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="C28">
-        <v>1530.6</v>
+        <v>1293</v>
       </c>
       <c r="D28">
-        <v>1538.9</v>
+        <v>1298.5</v>
       </c>
       <c r="E28">
-        <v>8.300000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="F28">
-        <v>96.36</v>
+        <v>94.48</v>
       </c>
       <c r="G28">
-        <v>92.47</v>
+        <v>89.70999999999999</v>
       </c>
       <c r="H28">
-        <v>0.57</v>
+        <v>0.7</v>
       </c>
       <c r="I28">
-        <v>0.04</v>
+        <v>0.54</v>
       </c>
       <c r="J28">
-        <v>3.89</v>
+        <v>4.77</v>
       </c>
       <c r="K28">
-        <v>0.53</v>
+        <v>0.17</v>
       </c>
       <c r="L28">
-        <v>2.03</v>
+        <v>1.24</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -10870,40 +10924,40 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>218</v>
       </c>
       <c r="C29">
-        <v>5833</v>
+        <v>1776.8</v>
       </c>
       <c r="D29">
-        <v>5875.5</v>
+        <v>1783.8</v>
       </c>
       <c r="E29">
-        <v>42.5</v>
+        <v>7</v>
       </c>
       <c r="F29">
-        <v>95.62</v>
+        <v>93.45999999999999</v>
       </c>
       <c r="G29">
-        <v>94.42</v>
+        <v>91.98</v>
       </c>
       <c r="H29">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="I29">
-        <v>-0.12</v>
+        <v>0.43</v>
       </c>
       <c r="J29">
-        <v>1.2</v>
+        <v>1.48</v>
       </c>
       <c r="K29">
-        <v>0.8</v>
+        <v>0.16</v>
       </c>
       <c r="L29">
-        <v>4.24</v>
+        <v>5.32</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -10914,37 +10968,37 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C30">
-        <v>3119.2</v>
+        <v>1494.7</v>
       </c>
       <c r="D30">
-        <v>3135.5</v>
+        <v>1502.1</v>
       </c>
       <c r="E30">
-        <v>16.3</v>
+        <v>7.4</v>
       </c>
       <c r="F30">
-        <v>97.06999999999999</v>
+        <v>98.17</v>
       </c>
       <c r="G30">
-        <v>93.06</v>
+        <v>89.17</v>
       </c>
       <c r="H30">
-        <v>0.73</v>
+        <v>0.68</v>
       </c>
       <c r="I30">
-        <v>0.37</v>
+        <v>0.53</v>
       </c>
       <c r="J30">
-        <v>4.01</v>
+        <v>9</v>
       </c>
       <c r="K30">
-        <v>0.36</v>
+        <v>0.15</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>3.27</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -10952,40 +11006,40 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="C31">
-        <v>1494.7</v>
+        <v>1881.5</v>
       </c>
       <c r="D31">
-        <v>1502.1</v>
+        <v>1891.7</v>
       </c>
       <c r="E31">
-        <v>7.4</v>
+        <v>10.2</v>
       </c>
       <c r="F31">
-        <v>98.17</v>
+        <v>97.52</v>
       </c>
       <c r="G31">
-        <v>89.17</v>
+        <v>94.23999999999999</v>
       </c>
       <c r="H31">
-        <v>0.68</v>
+        <v>0.74</v>
       </c>
       <c r="I31">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="J31">
-        <v>9</v>
+        <v>3.28</v>
       </c>
       <c r="K31">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="L31">
-        <v>3.27</v>
+        <v>3.66</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -10993,40 +11047,40 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>221</v>
       </c>
       <c r="C32">
-        <v>4311.3</v>
+        <v>1266.3</v>
       </c>
       <c r="D32">
-        <v>4341.3</v>
+        <v>1273.1</v>
       </c>
       <c r="E32">
-        <v>30</v>
+        <v>6.8</v>
       </c>
       <c r="F32">
-        <v>92.25</v>
+        <v>96.06999999999999</v>
       </c>
       <c r="G32">
-        <v>90.5</v>
+        <v>92.89</v>
       </c>
       <c r="H32">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="I32">
-        <v>0.36</v>
+        <v>0.61</v>
       </c>
       <c r="J32">
-        <v>1.75</v>
+        <v>3.18</v>
       </c>
       <c r="K32">
-        <v>0.26</v>
+        <v>0.14</v>
       </c>
       <c r="L32">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -11034,40 +11088,40 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C33">
-        <v>3181.1</v>
+        <v>9867</v>
       </c>
       <c r="D33">
-        <v>3200.7</v>
+        <v>9916</v>
       </c>
       <c r="E33">
-        <v>19.6</v>
+        <v>49</v>
       </c>
       <c r="F33">
-        <v>97.68000000000001</v>
+        <v>90.81</v>
       </c>
       <c r="G33">
-        <v>90.34</v>
+        <v>88.48999999999999</v>
       </c>
       <c r="H33">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="I33">
-        <v>0.6</v>
+        <v>0.53</v>
       </c>
       <c r="J33">
-        <v>7.34</v>
+        <v>2.32</v>
       </c>
       <c r="K33">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="L33">
-        <v>2.3</v>
+        <v>8.23</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -11075,40 +11129,40 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="C34">
-        <v>3996.7</v>
+        <v>117.59</v>
       </c>
       <c r="D34">
-        <v>4021.3</v>
+        <v>118.4</v>
       </c>
       <c r="E34">
-        <v>24.6</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F34">
-        <v>97.11</v>
+        <v>97.47</v>
       </c>
       <c r="G34">
-        <v>88.88</v>
+        <v>92.75</v>
       </c>
       <c r="H34">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="I34">
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
       <c r="J34">
-        <v>8.23</v>
+        <v>4.72</v>
       </c>
       <c r="K34">
-        <v>0.2</v>
+        <v>0.13</v>
       </c>
       <c r="L34">
-        <v>0.6</v>
+        <v>6.6</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -11116,40 +11170,40 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>177</v>
+        <v>60</v>
       </c>
       <c r="C35">
-        <v>749.7</v>
+        <v>839.9</v>
       </c>
       <c r="D35">
-        <v>755.45</v>
+        <v>844.05</v>
       </c>
       <c r="E35">
-        <v>5.75</v>
+        <v>4.15</v>
       </c>
       <c r="F35">
-        <v>95.29000000000001</v>
+        <v>93.55</v>
       </c>
       <c r="G35">
-        <v>94.01000000000001</v>
+        <v>92.61</v>
       </c>
       <c r="H35">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="I35">
-        <v>0.36</v>
+        <v>0.6</v>
       </c>
       <c r="J35">
-        <v>1.28</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="K35">
-        <v>0.44</v>
+        <v>0.13</v>
       </c>
       <c r="L35">
-        <v>6.7</v>
+        <v>5.02</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -11157,40 +11211,40 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="C36">
-        <v>253.97</v>
+        <v>612.25</v>
       </c>
       <c r="D36">
-        <v>255.7</v>
+        <v>615.85</v>
       </c>
       <c r="E36">
-        <v>1.73</v>
+        <v>3.6</v>
       </c>
       <c r="F36">
-        <v>93.29000000000001</v>
+        <v>98.11</v>
       </c>
       <c r="G36">
-        <v>91.56999999999999</v>
+        <v>94.04000000000001</v>
       </c>
       <c r="H36">
-        <v>0.78</v>
+        <v>0.66</v>
       </c>
       <c r="I36">
-        <v>0.39</v>
+        <v>0.54</v>
       </c>
       <c r="J36">
-        <v>1.72</v>
+        <v>4.08</v>
       </c>
       <c r="K36">
-        <v>0.39</v>
+        <v>0.12</v>
       </c>
       <c r="L36">
-        <v>7.27</v>
+        <v>1.96</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -11198,40 +11252,40 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="C37">
-        <v>455.25</v>
+        <v>2042.3</v>
       </c>
       <c r="D37">
-        <v>458.5</v>
+        <v>2055.1</v>
       </c>
       <c r="E37">
-        <v>3.25</v>
+        <v>12.8</v>
       </c>
       <c r="F37">
-        <v>97.48999999999999</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="G37">
-        <v>85.48</v>
+        <v>94.22</v>
       </c>
       <c r="H37">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="I37">
-        <v>0.39</v>
+        <v>0.55</v>
       </c>
       <c r="J37">
-        <v>12.01</v>
+        <v>1.18</v>
       </c>
       <c r="K37">
-        <v>0.27</v>
+        <v>0.12</v>
       </c>
       <c r="L37">
-        <v>0.6899999999999999</v>
+        <v>6.44</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -11239,40 +11293,40 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>190</v>
+        <v>102</v>
       </c>
       <c r="C38">
-        <v>164.12</v>
+        <v>1177.7</v>
       </c>
       <c r="D38">
-        <v>164.95</v>
+        <v>1183.6</v>
       </c>
       <c r="E38">
-        <v>0.83</v>
+        <v>5.9</v>
       </c>
       <c r="F38">
-        <v>87.92</v>
+        <v>97.88</v>
       </c>
       <c r="G38">
-        <v>83.56999999999999</v>
+        <v>96.76000000000001</v>
       </c>
       <c r="H38">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="I38">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="J38">
-        <v>4.34</v>
+        <v>1.13</v>
       </c>
       <c r="K38">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="L38">
-        <v>6.21</v>
+        <v>0.75</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -11280,40 +11334,40 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="C39">
-        <v>117.59</v>
+        <v>3181.1</v>
       </c>
       <c r="D39">
-        <v>118.4</v>
+        <v>3200.7</v>
       </c>
       <c r="E39">
-        <v>0.8100000000000001</v>
+        <v>19.6</v>
       </c>
       <c r="F39">
-        <v>97.47</v>
+        <v>97.68000000000001</v>
       </c>
       <c r="G39">
-        <v>92.75</v>
+        <v>90.34</v>
       </c>
       <c r="H39">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="I39">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="J39">
-        <v>4.72</v>
+        <v>7.34</v>
       </c>
       <c r="K39">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="L39">
-        <v>6.6</v>
+        <v>2.3</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -11321,37 +11375,37 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="C40">
-        <v>287.25</v>
+        <v>3855.1</v>
       </c>
       <c r="D40">
-        <v>288.55</v>
+        <v>3881.6</v>
       </c>
       <c r="E40">
-        <v>1.3</v>
+        <v>26.5</v>
       </c>
       <c r="F40">
-        <v>93.03</v>
+        <v>94.91</v>
       </c>
       <c r="G40">
-        <v>90.34</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="H40">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="I40">
-        <v>0.55</v>
+        <v>0.48</v>
       </c>
       <c r="J40">
-        <v>2.68</v>
+        <v>1.31</v>
       </c>
       <c r="K40">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="L40">
         <v>3.72</v>
@@ -11362,40 +11416,40 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>53</v>
       </c>
       <c r="C41">
-        <v>147.21</v>
+        <v>110.21</v>
       </c>
       <c r="D41">
-        <v>148.23</v>
+        <v>110.99</v>
       </c>
       <c r="E41">
-        <v>1.02</v>
+        <v>0.78</v>
       </c>
       <c r="F41">
-        <v>95.48</v>
+        <v>96.47</v>
       </c>
       <c r="G41">
-        <v>95.47</v>
+        <v>96.2</v>
       </c>
       <c r="H41">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="I41">
-        <v>0.65</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J41">
-        <v>0.02</v>
+        <v>0.27</v>
       </c>
       <c r="K41">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="L41">
-        <v>4.34</v>
+        <v>3.02</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -11403,40 +11457,40 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>207</v>
+        <v>82</v>
       </c>
       <c r="C42">
-        <v>5701</v>
+        <v>1011.6</v>
       </c>
       <c r="D42">
-        <v>5729.5</v>
+        <v>1017.3</v>
       </c>
       <c r="E42">
-        <v>28.5</v>
+        <v>5.7</v>
       </c>
       <c r="F42">
-        <v>97.06999999999999</v>
+        <v>94.45</v>
       </c>
       <c r="G42">
-        <v>93.84999999999999</v>
+        <v>94.18000000000001</v>
       </c>
       <c r="H42">
-        <v>0.59</v>
+        <v>0.75</v>
       </c>
       <c r="I42">
-        <v>0.22</v>
+        <v>0.67</v>
       </c>
       <c r="J42">
-        <v>3.22</v>
+        <v>0.26</v>
       </c>
       <c r="K42">
-        <v>0.37</v>
+        <v>0.08</v>
       </c>
       <c r="L42">
-        <v>4.95</v>
+        <v>0.74</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -11444,40 +11498,40 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>213</v>
+        <v>69</v>
       </c>
       <c r="C43">
-        <v>1881.5</v>
+        <v>570.35</v>
       </c>
       <c r="D43">
-        <v>1891.7</v>
+        <v>573.4</v>
       </c>
       <c r="E43">
-        <v>10.2</v>
+        <v>3.05</v>
       </c>
       <c r="F43">
-        <v>97.52</v>
+        <v>95.97</v>
       </c>
       <c r="G43">
-        <v>94.23999999999999</v>
+        <v>94.58</v>
       </c>
       <c r="H43">
-        <v>0.74</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I43">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="J43">
-        <v>3.28</v>
+        <v>1.39</v>
       </c>
       <c r="K43">
-        <v>0.14</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="L43">
-        <v>3.66</v>
+        <v>0.89</v>
       </c>
       <c r="M43">
         <v>0</v>
@@ -11485,40 +11539,40 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="C44">
-        <v>977.55</v>
+        <v>164.12</v>
       </c>
       <c r="D44">
-        <v>982.6</v>
+        <v>164.95</v>
       </c>
       <c r="E44">
-        <v>5.05</v>
+        <v>0.83</v>
       </c>
       <c r="F44">
-        <v>90.29000000000001</v>
+        <v>87.92</v>
       </c>
       <c r="G44">
-        <v>89.87</v>
+        <v>83.56999999999999</v>
       </c>
       <c r="H44">
-        <v>0.77</v>
+        <v>0.62</v>
       </c>
       <c r="I44">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J44">
-        <v>0.42</v>
+        <v>4.34</v>
       </c>
       <c r="K44">
-        <v>0.22</v>
+        <v>0.06</v>
       </c>
       <c r="L44">
-        <v>1.87</v>
+        <v>6.21</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -11526,40 +11580,40 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="C45">
-        <v>2042.3</v>
+        <v>10.05</v>
       </c>
       <c r="D45">
-        <v>2055.1</v>
+        <v>10.13</v>
       </c>
       <c r="E45">
-        <v>12.8</v>
+        <v>0.08</v>
       </c>
       <c r="F45">
-        <v>95.40000000000001</v>
+        <v>96.25</v>
       </c>
       <c r="G45">
-        <v>94.22</v>
+        <v>96.09</v>
       </c>
       <c r="H45">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
       <c r="I45">
-        <v>0.55</v>
+        <v>0.63</v>
       </c>
       <c r="J45">
-        <v>1.18</v>
+        <v>0.15</v>
       </c>
       <c r="K45">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="L45">
-        <v>6.44</v>
+        <v>6.46</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -11567,40 +11621,40 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="C46">
-        <v>1776.8</v>
+        <v>10.05</v>
       </c>
       <c r="D46">
-        <v>1783.8</v>
+        <v>10.13</v>
       </c>
       <c r="E46">
-        <v>7</v>
+        <v>0.08</v>
       </c>
       <c r="F46">
-        <v>93.45999999999999</v>
+        <v>96.25</v>
       </c>
       <c r="G46">
-        <v>91.98</v>
+        <v>96.09</v>
       </c>
       <c r="H46">
-        <v>0.59</v>
+        <v>0.7</v>
       </c>
       <c r="I46">
-        <v>0.43</v>
+        <v>0.63</v>
       </c>
       <c r="J46">
-        <v>1.48</v>
+        <v>0.15</v>
       </c>
       <c r="K46">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="L46">
-        <v>5.32</v>
+        <v>6.46</v>
       </c>
       <c r="M46">
         <v>0</v>
@@ -11608,40 +11662,40 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="C47">
-        <v>1266.3</v>
+        <v>838.25</v>
       </c>
       <c r="D47">
-        <v>1273.1</v>
+        <v>843.45</v>
       </c>
       <c r="E47">
-        <v>6.8</v>
+        <v>5.2</v>
       </c>
       <c r="F47">
-        <v>96.06999999999999</v>
+        <v>95.7</v>
       </c>
       <c r="G47">
-        <v>92.89</v>
+        <v>95.58</v>
       </c>
       <c r="H47">
-        <v>0.75</v>
+        <v>0.47</v>
       </c>
       <c r="I47">
-        <v>0.61</v>
+        <v>0.42</v>
       </c>
       <c r="J47">
-        <v>3.18</v>
+        <v>0.12</v>
       </c>
       <c r="K47">
-        <v>0.14</v>
+        <v>0.05</v>
       </c>
       <c r="L47">
-        <v>1.6</v>
+        <v>15.83</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -11649,40 +11703,40 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="C48">
-        <v>230.76</v>
+        <v>287.25</v>
       </c>
       <c r="D48">
-        <v>232.28</v>
+        <v>288.55</v>
       </c>
       <c r="E48">
-        <v>1.52</v>
+        <v>1.3</v>
       </c>
       <c r="F48">
-        <v>96.81</v>
+        <v>93.03</v>
       </c>
       <c r="G48">
-        <v>92.18000000000001</v>
+        <v>90.34</v>
       </c>
       <c r="H48">
-        <v>0.76</v>
+        <v>0.59</v>
       </c>
       <c r="I48">
-        <v>0.45</v>
+        <v>0.55</v>
       </c>
       <c r="J48">
-        <v>4.64</v>
+        <v>2.68</v>
       </c>
       <c r="K48">
-        <v>0.31</v>
+        <v>0.04</v>
       </c>
       <c r="L48">
-        <v>2.14</v>
+        <v>3.72</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -11690,40 +11744,40 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>235</v>
+        <v>107</v>
       </c>
       <c r="C49">
-        <v>1731.7</v>
+        <v>345.45</v>
       </c>
       <c r="D49">
-        <v>1739.2</v>
+        <v>347.1</v>
       </c>
       <c r="E49">
-        <v>7.5</v>
+        <v>1.65</v>
       </c>
       <c r="F49">
-        <v>95.27</v>
+        <v>98.36</v>
       </c>
       <c r="G49">
-        <v>90.97</v>
+        <v>95.29000000000001</v>
       </c>
       <c r="H49">
-        <v>0.7</v>
+        <v>0.59</v>
       </c>
       <c r="I49">
-        <v>0.49</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J49">
-        <v>4.29</v>
+        <v>3.07</v>
       </c>
       <c r="K49">
-        <v>0.2</v>
+        <v>0.03</v>
       </c>
       <c r="L49">
-        <v>1.75</v>
+        <v>10.51</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -11731,40 +11785,40 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="C50">
-        <v>10.05</v>
+        <v>147.21</v>
       </c>
       <c r="D50">
-        <v>10.13</v>
+        <v>148.23</v>
       </c>
       <c r="E50">
-        <v>0.08</v>
+        <v>1.02</v>
       </c>
       <c r="F50">
-        <v>96.25</v>
+        <v>95.48</v>
       </c>
       <c r="G50">
-        <v>96.09</v>
+        <v>95.47</v>
       </c>
       <c r="H50">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="I50">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="J50">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="K50">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="L50">
-        <v>6.46</v>
+        <v>4.34</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -11772,40 +11826,40 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>241</v>
+        <v>81</v>
       </c>
       <c r="C51">
-        <v>10.05</v>
+        <v>971.5</v>
       </c>
       <c r="D51">
-        <v>10.13</v>
+        <v>977.15</v>
       </c>
       <c r="E51">
-        <v>0.08</v>
+        <v>5.65</v>
       </c>
       <c r="F51">
-        <v>96.25</v>
+        <v>98.44</v>
       </c>
       <c r="G51">
-        <v>96.09</v>
+        <v>96.68000000000001</v>
       </c>
       <c r="H51">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="I51">
         <v>0.63</v>
       </c>
       <c r="J51">
-        <v>0.15</v>
+        <v>1.76</v>
       </c>
       <c r="K51">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="L51">
-        <v>6.46</v>
+        <v>5.46</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -11862,16 +11916,34 @@
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>246</v>
       </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
@@ -11921,40 +11993,40 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="C6">
-        <v>7138</v>
+        <v>1120</v>
       </c>
       <c r="D6">
-        <v>6941</v>
+        <v>1124.7</v>
       </c>
       <c r="E6">
-        <v>-197</v>
+        <v>4.7</v>
       </c>
       <c r="F6">
-        <v>90.19</v>
+        <v>80.86</v>
       </c>
       <c r="G6">
-        <v>89.58</v>
+        <v>73.15000000000001</v>
       </c>
       <c r="H6">
-        <v>-3.05</v>
+        <v>0.28</v>
       </c>
       <c r="I6">
-        <v>-0.72</v>
+        <v>0.38</v>
       </c>
       <c r="J6">
-        <v>0.61</v>
+        <v>7.71</v>
       </c>
       <c r="K6">
-        <v>-2.33</v>
+        <v>-0.1</v>
       </c>
       <c r="L6">
-        <v>-16.28</v>
+        <v>-4.42</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -11962,40 +12034,40 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>217</v>
       </c>
       <c r="C7">
-        <v>1120</v>
+        <v>184.87</v>
       </c>
       <c r="D7">
-        <v>1124.7</v>
+        <v>185.4</v>
       </c>
       <c r="E7">
-        <v>4.7</v>
+        <v>0.53</v>
       </c>
       <c r="F7">
-        <v>80.86</v>
+        <v>94.88</v>
       </c>
       <c r="G7">
-        <v>73.15000000000001</v>
+        <v>88.66</v>
       </c>
       <c r="H7">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="I7">
-        <v>0.38</v>
+        <v>0.54</v>
       </c>
       <c r="J7">
-        <v>7.71</v>
+        <v>6.22</v>
       </c>
       <c r="K7">
-        <v>-0.1</v>
+        <v>-0.18</v>
       </c>
       <c r="L7">
-        <v>-4.42</v>
+        <v>-8.529999999999999</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -12044,40 +12116,40 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="C9">
-        <v>184.87</v>
+        <v>308.25</v>
       </c>
       <c r="D9">
-        <v>185.4</v>
+        <v>310.25</v>
       </c>
       <c r="E9">
-        <v>0.53</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>94.88</v>
+        <v>89.66</v>
       </c>
       <c r="G9">
-        <v>88.66</v>
+        <v>85.58</v>
       </c>
       <c r="H9">
-        <v>0.36</v>
+        <v>0.76</v>
       </c>
       <c r="I9">
-        <v>0.54</v>
+        <v>0.93</v>
       </c>
       <c r="J9">
-        <v>6.22</v>
+        <v>4.08</v>
       </c>
       <c r="K9">
-        <v>-0.18</v>
+        <v>-0.17</v>
       </c>
       <c r="L9">
-        <v>-8.529999999999999</v>
+        <v>-5.18</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -12126,40 +12198,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>61</v>
       </c>
       <c r="C11">
-        <v>308.25</v>
+        <v>7138</v>
       </c>
       <c r="D11">
-        <v>310.25</v>
+        <v>6941</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>-197</v>
       </c>
       <c r="F11">
-        <v>89.66</v>
+        <v>90.19</v>
       </c>
       <c r="G11">
-        <v>85.58</v>
+        <v>89.58</v>
       </c>
       <c r="H11">
-        <v>0.76</v>
+        <v>-3.05</v>
       </c>
       <c r="I11">
-        <v>0.93</v>
+        <v>-0.72</v>
       </c>
       <c r="J11">
-        <v>4.08</v>
+        <v>0.61</v>
       </c>
       <c r="K11">
-        <v>-0.17</v>
+        <v>-2.33</v>
       </c>
       <c r="L11">
-        <v>-5.18</v>
+        <v>-16.28</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -12216,16 +12288,34 @@
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>246</v>
       </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
@@ -12316,40 +12406,40 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C7">
-        <v>145.83</v>
+        <v>282.9</v>
       </c>
       <c r="D7">
-        <v>146.49</v>
+        <v>284.7</v>
       </c>
       <c r="E7">
-        <v>0.66</v>
+        <v>1.8</v>
       </c>
       <c r="F7">
-        <v>91.67</v>
+        <v>88.13</v>
       </c>
       <c r="G7">
-        <v>93.51000000000001</v>
+        <v>92.64</v>
       </c>
       <c r="H7">
-        <v>0.33</v>
+        <v>0.51</v>
       </c>
       <c r="I7">
-        <v>-0.19</v>
+        <v>0.46</v>
       </c>
       <c r="J7">
-        <v>-1.84</v>
+        <v>-4.51</v>
       </c>
       <c r="K7">
-        <v>0.52</v>
+        <v>0.05</v>
       </c>
       <c r="L7">
-        <v>4.09</v>
+        <v>19.2</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -12357,40 +12447,40 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="C8">
-        <v>1409.7</v>
+        <v>2840.6</v>
       </c>
       <c r="D8">
-        <v>1418.3</v>
+        <v>2857.3</v>
       </c>
       <c r="E8">
-        <v>8.6</v>
+        <v>16.7</v>
       </c>
       <c r="F8">
-        <v>87.91</v>
+        <v>79.81</v>
       </c>
       <c r="G8">
-        <v>92.15000000000001</v>
+        <v>84.34</v>
       </c>
       <c r="H8">
-        <v>0.54</v>
+        <v>0.64</v>
       </c>
       <c r="I8">
-        <v>0.18</v>
+        <v>0.61</v>
       </c>
       <c r="J8">
-        <v>-4.24</v>
+        <v>-4.53</v>
       </c>
       <c r="K8">
-        <v>0.36</v>
+        <v>0.03</v>
       </c>
       <c r="L8">
-        <v>7.77</v>
+        <v>17.39</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -12398,40 +12488,40 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C9">
-        <v>7218.5</v>
+        <v>2875.8</v>
       </c>
       <c r="D9">
-        <v>7238</v>
+        <v>2890.4</v>
       </c>
       <c r="E9">
-        <v>19.5</v>
+        <v>14.6</v>
       </c>
       <c r="F9">
-        <v>85.68000000000001</v>
+        <v>80.68000000000001</v>
       </c>
       <c r="G9">
-        <v>90.48</v>
+        <v>91.12</v>
       </c>
       <c r="H9">
-        <v>0.58</v>
+        <v>0.75</v>
       </c>
       <c r="I9">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
       <c r="J9">
-        <v>-4.8</v>
+        <v>-10.44</v>
       </c>
       <c r="K9">
-        <v>0.28</v>
+        <v>0.38</v>
       </c>
       <c r="L9">
-        <v>3.08</v>
+        <v>14.61</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -12439,40 +12529,40 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="C10">
-        <v>501.3</v>
+        <v>104.21</v>
       </c>
       <c r="D10">
-        <v>504.05</v>
+        <v>104.74</v>
       </c>
       <c r="E10">
-        <v>2.75</v>
+        <v>0.53</v>
       </c>
       <c r="F10">
-        <v>85.89</v>
+        <v>86.06999999999999</v>
       </c>
       <c r="G10">
-        <v>91.44</v>
+        <v>96.36</v>
       </c>
       <c r="H10">
-        <v>0.6899999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="I10">
-        <v>0.2</v>
+        <v>0.63</v>
       </c>
       <c r="J10">
-        <v>-5.55</v>
+        <v>-10.29</v>
       </c>
       <c r="K10">
-        <v>0.48</v>
+        <v>0.09</v>
       </c>
       <c r="L10">
-        <v>3.5</v>
+        <v>12.43</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -12480,40 +12570,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="C11">
-        <v>944.05</v>
+        <v>296.9</v>
       </c>
       <c r="D11">
-        <v>947.3</v>
+        <v>299</v>
       </c>
       <c r="E11">
-        <v>3.25</v>
+        <v>2.1</v>
       </c>
       <c r="F11">
-        <v>93.31999999999999</v>
+        <v>78.48999999999999</v>
       </c>
       <c r="G11">
-        <v>93.92</v>
+        <v>89.66</v>
       </c>
       <c r="H11">
-        <v>0.61</v>
+        <v>0.57</v>
       </c>
       <c r="I11">
-        <v>0.27</v>
+        <v>0.36</v>
       </c>
       <c r="J11">
-        <v>-0.6</v>
+        <v>-11.16</v>
       </c>
       <c r="K11">
-        <v>0.34</v>
+        <v>0.21</v>
       </c>
       <c r="L11">
-        <v>7.29</v>
+        <v>10.64</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -12521,40 +12611,40 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="C12">
-        <v>2875.8</v>
+        <v>1208</v>
       </c>
       <c r="D12">
-        <v>2890.4</v>
+        <v>1215.7</v>
       </c>
       <c r="E12">
-        <v>14.6</v>
+        <v>7.7</v>
       </c>
       <c r="F12">
-        <v>80.68000000000001</v>
+        <v>95.98</v>
       </c>
       <c r="G12">
-        <v>91.12</v>
+        <v>96.05</v>
       </c>
       <c r="H12">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="I12">
-        <v>0.37</v>
+        <v>0.61</v>
       </c>
       <c r="J12">
-        <v>-10.44</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="K12">
-        <v>0.38</v>
+        <v>0.13</v>
       </c>
       <c r="L12">
-        <v>14.61</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -12562,40 +12652,40 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C13">
-        <v>5867</v>
+        <v>557.4</v>
       </c>
       <c r="D13">
-        <v>5892</v>
+        <v>560</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>2.6</v>
       </c>
       <c r="F13">
-        <v>89.26000000000001</v>
+        <v>94.03</v>
       </c>
       <c r="G13">
-        <v>94.92</v>
+        <v>94.38</v>
       </c>
       <c r="H13">
-        <v>0.43</v>
+        <v>0.73</v>
       </c>
       <c r="I13">
-        <v>0.29</v>
+        <v>0.52</v>
       </c>
       <c r="J13">
-        <v>-5.67</v>
+        <v>-0.36</v>
       </c>
       <c r="K13">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="L13">
-        <v>0.1</v>
+        <v>8.49</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -12603,40 +12693,40 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="C14">
-        <v>514.4</v>
+        <v>1409.7</v>
       </c>
       <c r="D14">
-        <v>517.7</v>
+        <v>1418.3</v>
       </c>
       <c r="E14">
-        <v>3.3</v>
+        <v>8.6</v>
       </c>
       <c r="F14">
-        <v>80.56999999999999</v>
+        <v>87.91</v>
       </c>
       <c r="G14">
-        <v>93.65000000000001</v>
+        <v>92.15000000000001</v>
       </c>
       <c r="H14">
         <v>0.54</v>
       </c>
       <c r="I14">
-        <v>0.31</v>
+        <v>0.18</v>
       </c>
       <c r="J14">
-        <v>-13.08</v>
+        <v>-4.24</v>
       </c>
       <c r="K14">
-        <v>0.23</v>
+        <v>0.36</v>
       </c>
       <c r="L14">
-        <v>2.19</v>
+        <v>7.77</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -12644,40 +12734,40 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C15">
-        <v>1430.4</v>
+        <v>944.05</v>
       </c>
       <c r="D15">
-        <v>1437.6</v>
+        <v>947.3</v>
       </c>
       <c r="E15">
-        <v>7.2</v>
+        <v>3.25</v>
       </c>
       <c r="F15">
-        <v>93.45</v>
+        <v>93.31999999999999</v>
       </c>
       <c r="G15">
-        <v>94.70999999999999</v>
+        <v>93.92</v>
       </c>
       <c r="H15">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="I15">
-        <v>0.55</v>
+        <v>0.27</v>
       </c>
       <c r="J15">
-        <v>-1.26</v>
+        <v>-0.6</v>
       </c>
       <c r="K15">
-        <v>0.09</v>
+        <v>0.34</v>
       </c>
       <c r="L15">
-        <v>5.81</v>
+        <v>7.29</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -12685,40 +12775,40 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C16">
-        <v>2840.6</v>
+        <v>1430.4</v>
       </c>
       <c r="D16">
-        <v>2857.3</v>
+        <v>1437.6</v>
       </c>
       <c r="E16">
-        <v>16.7</v>
+        <v>7.2</v>
       </c>
       <c r="F16">
-        <v>79.81</v>
+        <v>93.45</v>
       </c>
       <c r="G16">
-        <v>84.34</v>
+        <v>94.70999999999999</v>
       </c>
       <c r="H16">
         <v>0.64</v>
       </c>
       <c r="I16">
-        <v>0.61</v>
+        <v>0.55</v>
       </c>
       <c r="J16">
-        <v>-4.53</v>
+        <v>-1.26</v>
       </c>
       <c r="K16">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="L16">
-        <v>17.39</v>
+        <v>5.81</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -12726,40 +12816,40 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="C17">
-        <v>557.4</v>
+        <v>983.6</v>
       </c>
       <c r="D17">
-        <v>560</v>
+        <v>988.45</v>
       </c>
       <c r="E17">
-        <v>2.6</v>
+        <v>4.85</v>
       </c>
       <c r="F17">
-        <v>94.03</v>
+        <v>89.65000000000001</v>
       </c>
       <c r="G17">
-        <v>94.38</v>
+        <v>91.13</v>
       </c>
       <c r="H17">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="I17">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="J17">
-        <v>-0.36</v>
+        <v>-1.48</v>
       </c>
       <c r="K17">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="L17">
-        <v>8.49</v>
+        <v>5.74</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -12767,40 +12857,40 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="C18">
-        <v>296.9</v>
+        <v>3745.2</v>
       </c>
       <c r="D18">
-        <v>299</v>
+        <v>3769.6</v>
       </c>
       <c r="E18">
-        <v>2.1</v>
+        <v>24.4</v>
       </c>
       <c r="F18">
-        <v>78.48999999999999</v>
+        <v>94.52</v>
       </c>
       <c r="G18">
-        <v>89.66</v>
+        <v>94.65000000000001</v>
       </c>
       <c r="H18">
-        <v>0.57</v>
+        <v>0.71</v>
       </c>
       <c r="I18">
-        <v>0.36</v>
+        <v>0.43</v>
       </c>
       <c r="J18">
-        <v>-11.16</v>
+        <v>-0.13</v>
       </c>
       <c r="K18">
-        <v>0.21</v>
+        <v>0.27</v>
       </c>
       <c r="L18">
-        <v>10.64</v>
+        <v>4.72</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -12808,40 +12898,40 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="C19">
-        <v>245.64</v>
+        <v>403.6</v>
       </c>
       <c r="D19">
-        <v>246.02</v>
+        <v>406.5</v>
       </c>
       <c r="E19">
-        <v>0.38</v>
+        <v>2.9</v>
       </c>
       <c r="F19">
-        <v>90.03</v>
+        <v>91.92</v>
       </c>
       <c r="G19">
-        <v>92.64</v>
+        <v>96.06999999999999</v>
       </c>
       <c r="H19">
-        <v>-0.07000000000000001</v>
+        <v>0.61</v>
       </c>
       <c r="I19">
-        <v>-0.11</v>
+        <v>0.6</v>
       </c>
       <c r="J19">
-        <v>-2.61</v>
+        <v>-4.15</v>
       </c>
       <c r="K19">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="L19">
-        <v>1.34</v>
+        <v>4.59</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -12849,40 +12939,40 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>282.9</v>
+        <v>145.83</v>
       </c>
       <c r="D20">
-        <v>284.7</v>
+        <v>146.49</v>
       </c>
       <c r="E20">
-        <v>1.8</v>
+        <v>0.66</v>
       </c>
       <c r="F20">
-        <v>88.13</v>
+        <v>91.67</v>
       </c>
       <c r="G20">
-        <v>92.64</v>
+        <v>93.51000000000001</v>
       </c>
       <c r="H20">
-        <v>0.51</v>
+        <v>0.33</v>
       </c>
       <c r="I20">
-        <v>0.46</v>
+        <v>-0.19</v>
       </c>
       <c r="J20">
-        <v>-4.51</v>
+        <v>-1.84</v>
       </c>
       <c r="K20">
-        <v>0.05</v>
+        <v>0.52</v>
       </c>
       <c r="L20">
-        <v>19.2</v>
+        <v>4.09</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -12890,40 +12980,40 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="C21">
-        <v>104.21</v>
+        <v>1539.7</v>
       </c>
       <c r="D21">
-        <v>104.74</v>
+        <v>1547.6</v>
       </c>
       <c r="E21">
-        <v>0.53</v>
+        <v>7.9</v>
       </c>
       <c r="F21">
-        <v>86.06999999999999</v>
+        <v>92.42</v>
       </c>
       <c r="G21">
-        <v>96.36</v>
+        <v>94.53</v>
       </c>
       <c r="H21">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
       <c r="I21">
-        <v>0.63</v>
+        <v>0.55</v>
       </c>
       <c r="J21">
-        <v>-10.29</v>
+        <v>-2.11</v>
       </c>
       <c r="K21">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="L21">
-        <v>12.43</v>
+        <v>3.55</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -12931,40 +13021,40 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>54</v>
       </c>
       <c r="C22">
-        <v>132.25</v>
+        <v>501.3</v>
       </c>
       <c r="D22">
-        <v>132.8</v>
+        <v>504.05</v>
       </c>
       <c r="E22">
-        <v>0.55</v>
+        <v>2.75</v>
       </c>
       <c r="F22">
-        <v>90.42</v>
+        <v>85.89</v>
       </c>
       <c r="G22">
-        <v>92.64</v>
+        <v>91.44</v>
       </c>
       <c r="H22">
-        <v>0.66</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I22">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="J22">
-        <v>-2.23</v>
+        <v>-5.55</v>
       </c>
       <c r="K22">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
       <c r="L22">
-        <v>0.07000000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -12972,40 +13062,40 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>240</v>
       </c>
       <c r="C23">
-        <v>504.65</v>
+        <v>2161.6</v>
       </c>
       <c r="D23">
-        <v>507.65</v>
+        <v>2170.3</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F23">
-        <v>94.29000000000001</v>
+        <v>87.12</v>
       </c>
       <c r="G23">
-        <v>95.17</v>
+        <v>91.13</v>
       </c>
       <c r="H23">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
       <c r="I23">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="J23">
-        <v>-0.88</v>
+        <v>-4.02</v>
       </c>
       <c r="K23">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="L23">
-        <v>0.44</v>
+        <v>3.42</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -13013,40 +13103,40 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>49</v>
       </c>
       <c r="C24">
-        <v>180.22</v>
+        <v>7218.5</v>
       </c>
       <c r="D24">
-        <v>181.13</v>
+        <v>7238</v>
       </c>
       <c r="E24">
-        <v>0.91</v>
+        <v>19.5</v>
       </c>
       <c r="F24">
-        <v>89.5</v>
+        <v>85.68000000000001</v>
       </c>
       <c r="G24">
-        <v>92.94</v>
+        <v>90.48</v>
       </c>
       <c r="H24">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="I24">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="J24">
-        <v>-3.43</v>
+        <v>-4.8</v>
       </c>
       <c r="K24">
-        <v>0.1</v>
+        <v>0.28</v>
       </c>
       <c r="L24">
-        <v>0.99</v>
+        <v>3.08</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -13054,40 +13144,40 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C25">
-        <v>421.05</v>
+        <v>873.1</v>
       </c>
       <c r="D25">
-        <v>422.7</v>
+        <v>876.4</v>
       </c>
       <c r="E25">
-        <v>1.65</v>
+        <v>3.3</v>
       </c>
       <c r="F25">
-        <v>85.04000000000001</v>
+        <v>88.78</v>
       </c>
       <c r="G25">
-        <v>85.19</v>
+        <v>90.62</v>
       </c>
       <c r="H25">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="I25">
-        <v>0.22</v>
+        <v>-0.09</v>
       </c>
       <c r="J25">
-        <v>-0.15</v>
+        <v>-1.84</v>
       </c>
       <c r="K25">
-        <v>0.25</v>
+        <v>0.57</v>
       </c>
       <c r="L25">
-        <v>2.01</v>
+        <v>2.37</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -13095,40 +13185,40 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="C26">
-        <v>1539.7</v>
+        <v>514.4</v>
       </c>
       <c r="D26">
-        <v>1547.6</v>
+        <v>517.7</v>
       </c>
       <c r="E26">
-        <v>7.9</v>
+        <v>3.3</v>
       </c>
       <c r="F26">
-        <v>92.42</v>
+        <v>80.56999999999999</v>
       </c>
       <c r="G26">
-        <v>94.53</v>
+        <v>93.65000000000001</v>
       </c>
       <c r="H26">
-        <v>0.75</v>
+        <v>0.54</v>
       </c>
       <c r="I26">
-        <v>0.55</v>
+        <v>0.31</v>
       </c>
       <c r="J26">
-        <v>-2.11</v>
+        <v>-13.08</v>
       </c>
       <c r="K26">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="L26">
-        <v>3.55</v>
+        <v>2.19</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -13136,40 +13226,40 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C27">
-        <v>873.1</v>
+        <v>421.05</v>
       </c>
       <c r="D27">
-        <v>876.4</v>
+        <v>422.7</v>
       </c>
       <c r="E27">
-        <v>3.3</v>
+        <v>1.65</v>
       </c>
       <c r="F27">
-        <v>88.78</v>
+        <v>85.04000000000001</v>
       </c>
       <c r="G27">
-        <v>90.62</v>
+        <v>85.19</v>
       </c>
       <c r="H27">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="I27">
-        <v>-0.09</v>
+        <v>0.22</v>
       </c>
       <c r="J27">
-        <v>-1.84</v>
+        <v>-0.15</v>
       </c>
       <c r="K27">
-        <v>0.57</v>
+        <v>0.25</v>
       </c>
       <c r="L27">
-        <v>2.37</v>
+        <v>2.01</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -13177,40 +13267,40 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="C28">
-        <v>983.6</v>
+        <v>245.64</v>
       </c>
       <c r="D28">
-        <v>988.45</v>
+        <v>246.02</v>
       </c>
       <c r="E28">
-        <v>4.85</v>
+        <v>0.38</v>
       </c>
       <c r="F28">
-        <v>89.65000000000001</v>
+        <v>90.03</v>
       </c>
       <c r="G28">
-        <v>91.13</v>
+        <v>92.64</v>
       </c>
       <c r="H28">
-        <v>0.71</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I28">
-        <v>0.63</v>
+        <v>-0.11</v>
       </c>
       <c r="J28">
-        <v>-1.48</v>
+        <v>-2.61</v>
       </c>
       <c r="K28">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="L28">
-        <v>5.74</v>
+        <v>1.34</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -13218,40 +13308,40 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C29">
-        <v>1208</v>
+        <v>180.22</v>
       </c>
       <c r="D29">
-        <v>1215.7</v>
+        <v>181.13</v>
       </c>
       <c r="E29">
-        <v>7.7</v>
+        <v>0.91</v>
       </c>
       <c r="F29">
-        <v>95.98</v>
+        <v>89.5</v>
       </c>
       <c r="G29">
-        <v>96.05</v>
+        <v>92.94</v>
       </c>
       <c r="H29">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="I29">
-        <v>0.61</v>
+        <v>0.48</v>
       </c>
       <c r="J29">
-        <v>-0.07000000000000001</v>
+        <v>-3.43</v>
       </c>
       <c r="K29">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="L29">
-        <v>9.880000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -13259,40 +13349,40 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="C30">
-        <v>3745.2</v>
+        <v>504.65</v>
       </c>
       <c r="D30">
-        <v>3769.6</v>
+        <v>507.65</v>
       </c>
       <c r="E30">
-        <v>24.4</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>94.52</v>
+        <v>94.29000000000001</v>
       </c>
       <c r="G30">
-        <v>94.65000000000001</v>
+        <v>95.17</v>
       </c>
       <c r="H30">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="I30">
-        <v>0.43</v>
+        <v>0.55</v>
       </c>
       <c r="J30">
-        <v>-0.13</v>
+        <v>-0.88</v>
       </c>
       <c r="K30">
-        <v>0.27</v>
+        <v>0.12</v>
       </c>
       <c r="L30">
-        <v>4.72</v>
+        <v>0.44</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -13300,40 +13390,40 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>92</v>
       </c>
       <c r="C31">
-        <v>2161.6</v>
+        <v>5867</v>
       </c>
       <c r="D31">
-        <v>2170.3</v>
+        <v>5892</v>
       </c>
       <c r="E31">
-        <v>8.699999999999999</v>
+        <v>25</v>
       </c>
       <c r="F31">
-        <v>87.12</v>
+        <v>89.26000000000001</v>
       </c>
       <c r="G31">
-        <v>91.13</v>
+        <v>94.92</v>
       </c>
       <c r="H31">
-        <v>0.64</v>
+        <v>0.43</v>
       </c>
       <c r="I31">
-        <v>0.5</v>
+        <v>0.29</v>
       </c>
       <c r="J31">
-        <v>-4.02</v>
+        <v>-5.67</v>
       </c>
       <c r="K31">
         <v>0.14</v>
       </c>
       <c r="L31">
-        <v>3.42</v>
+        <v>0.1</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -13341,40 +13431,40 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="C32">
-        <v>403.6</v>
+        <v>132.25</v>
       </c>
       <c r="D32">
-        <v>406.5</v>
+        <v>132.8</v>
       </c>
       <c r="E32">
-        <v>2.9</v>
+        <v>0.55</v>
       </c>
       <c r="F32">
-        <v>91.92</v>
+        <v>90.42</v>
       </c>
       <c r="G32">
-        <v>96.06999999999999</v>
+        <v>92.64</v>
       </c>
       <c r="H32">
-        <v>0.61</v>
+        <v>0.66</v>
       </c>
       <c r="I32">
-        <v>0.6</v>
+        <v>0.26</v>
       </c>
       <c r="J32">
-        <v>-4.15</v>
+        <v>-2.23</v>
       </c>
       <c r="K32">
-        <v>0.01</v>
+        <v>0.4</v>
       </c>
       <c r="L32">
-        <v>4.59</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -13431,16 +13521,34 @@
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>246</v>
       </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
@@ -13531,40 +13639,40 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="C7">
-        <v>5775</v>
+        <v>361.4</v>
       </c>
       <c r="D7">
-        <v>5777</v>
+        <v>359.8</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>-1.6</v>
       </c>
       <c r="F7">
-        <v>92.91</v>
+        <v>92.67</v>
       </c>
       <c r="G7">
-        <v>94.65000000000001</v>
+        <v>93.14</v>
       </c>
       <c r="H7">
-        <v>0.09</v>
+        <v>-0.33</v>
       </c>
       <c r="I7">
-        <v>0.38</v>
+        <v>0.28</v>
       </c>
       <c r="J7">
-        <v>-1.74</v>
+        <v>-0.47</v>
       </c>
       <c r="K7">
-        <v>-0.29</v>
+        <v>-0.61</v>
       </c>
       <c r="L7">
-        <v>-0.59</v>
+        <v>-8.41</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -13654,40 +13762,40 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="C10">
-        <v>361.4</v>
+        <v>5070.5</v>
       </c>
       <c r="D10">
-        <v>359.8</v>
+        <v>5067</v>
       </c>
       <c r="E10">
-        <v>-1.6</v>
+        <v>-3.5</v>
       </c>
       <c r="F10">
-        <v>92.67</v>
+        <v>94.98</v>
       </c>
       <c r="G10">
-        <v>93.14</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="H10">
-        <v>-0.33</v>
+        <v>0.25</v>
       </c>
       <c r="I10">
-        <v>0.28</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J10">
-        <v>-0.47</v>
+        <v>-0.12</v>
       </c>
       <c r="K10">
-        <v>-0.61</v>
+        <v>-0.31</v>
       </c>
       <c r="L10">
-        <v>-8.41</v>
+        <v>-2.03</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -13695,40 +13803,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="C11">
-        <v>5070.5</v>
+        <v>5775</v>
       </c>
       <c r="D11">
-        <v>5067</v>
+        <v>5777</v>
       </c>
       <c r="E11">
-        <v>-3.5</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>94.98</v>
+        <v>92.91</v>
       </c>
       <c r="G11">
-        <v>95.09999999999999</v>
+        <v>94.65000000000001</v>
       </c>
       <c r="H11">
-        <v>0.25</v>
+        <v>0.09</v>
       </c>
       <c r="I11">
-        <v>0.5600000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="J11">
-        <v>-0.12</v>
+        <v>-1.74</v>
       </c>
       <c r="K11">
-        <v>-0.31</v>
+        <v>-0.29</v>
       </c>
       <c r="L11">
-        <v>-2.03</v>
+        <v>-0.59</v>
       </c>
       <c r="M11">
         <v>0</v>

</xml_diff>